<commit_message>
Add export of data associated with temporary user
</commit_message>
<xml_diff>
--- a/smapServer/WebContent/tasks_template.xlsx
+++ b/smapServer/WebContent/tasks_template.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="-2200" windowWidth="24480" windowHeight="13380"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14300"/>
   </bookViews>
   <sheets>
-    <sheet name="tasks" sheetId="1" r:id="rId1"/>
-    <sheet name="settings" sheetId="2" r:id="rId2"/>
+    <sheet name="Intro" sheetId="3" r:id="rId1"/>
+    <sheet name="tasks" sheetId="1" r:id="rId2"/>
+    <sheet name="settings" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>form</t>
   </si>
@@ -65,13 +66,85 @@
   </si>
   <si>
     <t>Australia/Melbourne</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Heading</t>
+  </si>
+  <si>
+    <t>Valid Values</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>The login id of a user</t>
+  </si>
+  <si>
+    <t>generate_user</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Can be left empty if generate_user is set to 'yes'</t>
+  </si>
+  <si>
+    <t>A temporary logon will be generated.  Ignored if the assignee_ident is set.</t>
+  </si>
+  <si>
+    <t>Or leave blank</t>
+  </si>
+  <si>
+    <t>generate_user_name</t>
+  </si>
+  <si>
+    <t>Users Name.  Any language</t>
+  </si>
+  <si>
+    <t>If generate_user is set to yes, and assignee_ident is not set then this will be used as the name of the generated user.</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>Read Only</t>
+  </si>
+  <si>
+    <t>If you enter a value in here it will be ignored.  However when the task list is downloaded from the server then the URL used to access this task will be set in this column</t>
+  </si>
+  <si>
+    <t>The users email</t>
+  </si>
+  <si>
+    <t>Used to send notifications to users.  Ignored if the assignee ident is set as the email of the user account will be used.</t>
+  </si>
+  <si>
+    <t>Display Name of the form  to complete as part of this task</t>
+  </si>
+  <si>
+    <t>Name of task</t>
+  </si>
+  <si>
+    <t>Status of task</t>
+  </si>
+  <si>
+    <t>The URL to complete the task in web forms</t>
+  </si>
+  <si>
+    <t>generated_user_name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -84,16 +157,89 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD85357"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE46769"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -101,15 +247,80 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -439,63 +650,186 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1"/>
+  <dimension ref="B2:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="13" width="20" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="17.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="78.33203125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="2:5" ht="15">
+      <c r="B2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+    </row>
+    <row r="3" spans="2:5" ht="15">
+      <c r="B3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="2:5" ht="15">
+      <c r="B4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="2:5" ht="15">
+      <c r="B5" s="2"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="2:5" ht="15">
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="15">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="2:5" ht="45">
+      <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="2:5" ht="15">
+      <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="2:5" ht="15">
+      <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="2:5" ht="15">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="2:5" ht="15">
+      <c r="B12" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="C12" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="15">
+      <c r="B14" s="13"/>
+      <c r="C14" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="12"/>
+      <c r="E14" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="28">
+      <c r="B15" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="28">
+      <c r="B16" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
+      <c r="C16" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+    </row>
+    <row r="18" spans="2:5" ht="28">
+      <c r="B18" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -506,6 +840,147 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="D27" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="16" width="20" style="6" customWidth="1"/>
+    <col min="17" max="16384" width="8.83203125" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="M2" s="11"/>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="M3" s="11"/>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="M4" s="11"/>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="M5" s="11"/>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="M6" s="11"/>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="M7" s="11"/>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="M8" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Changed column name in tasks template to "generated_user_name"
</commit_message>
<xml_diff>
--- a/smapServer/WebContent/tasks_template.xlsx
+++ b/smapServer/WebContent/tasks_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t>form</t>
   </si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>Or leave blank</t>
-  </si>
-  <si>
-    <t>generate_user_name</t>
   </si>
   <si>
     <t>Users Name.  Any language</t>
@@ -652,7 +649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -700,7 +697,7 @@
         <v>17</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>18</v>
@@ -717,7 +714,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="2"/>
@@ -727,7 +724,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -737,7 +734,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>21</v>
@@ -786,14 +783,14 @@
     </row>
     <row r="15" spans="2:5" ht="28">
       <c r="B15" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" s="13"/>
       <c r="E15" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="28">
@@ -801,11 +798,11 @@
         <v>9</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16" s="13"/>
       <c r="E16" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="2:5">
@@ -816,16 +813,16 @@
     </row>
     <row r="18" spans="2:5" ht="28">
       <c r="B18" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>21</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -842,11 +839,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D27" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -872,7 +869,7 @@
         <v>20</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>9</v>
@@ -893,7 +890,7 @@
         <v>8</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>10</v>

</xml_diff>